<commit_message>
se hace cambio del pdf de derechos y deveres del usuario
</commit_message>
<xml_diff>
--- a/src/Views/assets/excel/empleados_registro.xlsx
+++ b/src/Views/assets/excel/empleados_registro.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t xml:space="preserve">Relacion de Solicitudes</t>
+    <t xml:space="preserve">Registro de Empleados</t>
   </si>
   <si>
     <t>#</t>
@@ -138,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -156,8 +156,11 @@
     <xf fontId="2" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf fontId="2" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf fontId="2" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -757,25 +760,25 @@
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -797,7 +800,7 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="9"/>
+      <c r="D3" s="10"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -812,7 +815,7 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="9"/>
+      <c r="D4" s="10"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -827,7 +830,7 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="9"/>
+      <c r="D5" s="10"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -841,7 +844,7 @@
     <row r="6" ht="14.25">
       <c r="B6" s="1"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="9"/>
+      <c r="D6" s="10"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -855,7 +858,7 @@
     <row r="7" ht="14.25">
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="9"/>
+      <c r="D7" s="10"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -869,7 +872,7 @@
     <row r="8" ht="14.25">
       <c r="B8" s="1"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="9"/>
+      <c r="D8" s="10"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>

</xml_diff>